<commit_message>
Addition of profile templates
</commit_message>
<xml_diff>
--- a/Excel_profile_templates/Profile Template - CC RelatedPerson.xlsx
+++ b/Excel_profile_templates/Profile Template - CC RelatedPerson.xlsx
@@ -32,6 +32,21 @@
     <t>RelatedPerson</t>
   </si>
   <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>Mandatory</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>Not Used</t>
+  </si>
+  <si>
     <t>​</t>
   </si>
   <si>
@@ -42,25 +57,10 @@
 Constraint (dom-3): If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource</t>
   </si>
   <si>
-    <t>Select</t>
-  </si>
-  <si>
     <t>- id</t>
   </si>
   <si>
     <t>0..1</t>
-  </si>
-  <si>
-    <t>Mandatory</t>
-  </si>
-  <si>
-    <t>Required</t>
-  </si>
-  <si>
-    <t>Optional</t>
-  </si>
-  <si>
-    <t>Not Used</t>
   </si>
   <si>
     <t>Id</t>
@@ -328,7 +328,7 @@
     <t>A name associated with the person</t>
   </si>
   <si>
-    <t>usual | official | temp | nickname | anonymous | old | maiden
+    <t>usual : official : temp : nickname : anonymous : old : maiden
 Binding (required): The use of a human name [NameUse](http://hl7.org/fhir/stu3/valueset-name-use.html)</t>
   </si>
   <si>
@@ -373,14 +373,14 @@
 Constraint (cpt-2): A system is required if a value is provided.</t>
   </si>
   <si>
-    <t>phone | fax | email | pager | url | sms | other
+    <t>phone : fax : email : pager : url : sms : other
 Binding (required): Telecommunications form for contact point [ContactPointSystem](http://hl7.org/fhir/stu3/valueset-contact-point-system.html)</t>
   </si>
   <si>
     <t>The actual contact point details</t>
   </si>
   <si>
-    <t>home | work | temp | old | mobile - purpose of this contact point
+    <t>home : work : temp : old : mobile - purpose of this contact point
 Binding (required): Use of contact point [ContactPointUse](http://hl7.org/fhir/stu3/valueset-contact-point-use.html)</t>
   </si>
   <si>
@@ -400,7 +400,7 @@
     <t>- gender</t>
   </si>
   <si>
-    <t>male | female | other | unknown
+    <t>male : female : other : unknown
 Binding (required): The gender of a person used for administrative purposes. [AdministrativeGender](http://hl7.org/fhir/stu3/valueset-administrative-gender.html)</t>
   </si>
   <si>
@@ -422,11 +422,11 @@
     <t>Address where the related person can be contacted or visited</t>
   </si>
   <si>
-    <t>home | work | temp | old - purpose of this address
+    <t>home : work : temp : old - purpose of this address
 Binding (required): The use of an address [AddressUse](http://hl7.org/fhir/stu3/valueset-address-use.html)</t>
   </si>
   <si>
-    <t>postal | physical | both
+    <t>postal : physical : both
 Binding (required): The type of an address (physical / postal) [AddressType](http://hl7.org/fhir/stu3/valueset-address-type.html)</t>
   </si>
   <si>
@@ -577,6 +577,7 @@
     <font>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <sz val="8.0"/>
       <color rgb="FF333333"/>
@@ -588,7 +589,6 @@
       <color rgb="FF474747"/>
       <name val="Inherit"/>
     </font>
-    <font/>
     <font>
       <sz val="8.0"/>
       <color rgb="FF005EB8"/>
@@ -671,19 +671,19 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
@@ -709,10 +709,10 @@
     <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -794,78 +794,78 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>10</v>
+      <c r="B4" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>10</v>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>10</v>
+      <c r="B6" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>24</v>
@@ -875,36 +875,36 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>10</v>
+      <c r="B7" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="8" t="s">
         <v>32</v>
       </c>
     </row>
@@ -912,16 +912,16 @@
       <c r="A9" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="8" t="s">
         <v>35</v>
       </c>
     </row>
@@ -929,16 +929,16 @@
       <c r="A10" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="8" t="s">
         <v>38</v>
       </c>
     </row>
@@ -946,11 +946,11 @@
       <c r="A11" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>10</v>
+      <c r="B11" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>24</v>
@@ -963,11 +963,11 @@
       <c r="A12" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>10</v>
+      <c r="B12" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>42</v>
@@ -980,16 +980,16 @@
       <c r="A13" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="8" t="s">
         <v>46</v>
       </c>
     </row>
@@ -997,16 +997,16 @@
       <c r="A14" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>10</v>
+      <c r="B14" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="8" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1014,16 +1014,16 @@
       <c r="A15" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>10</v>
+      <c r="B15" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="8" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1031,16 +1031,16 @@
       <c r="A16" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>10</v>
+      <c r="B16" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="8" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1048,16 +1048,16 @@
       <c r="A17" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>10</v>
+      <c r="B17" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="8" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1065,16 +1065,16 @@
       <c r="A18" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>10</v>
+      <c r="B18" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="8" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1082,16 +1082,16 @@
       <c r="A19" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>10</v>
+      <c r="B19" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="8" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1099,16 +1099,16 @@
       <c r="A20" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>10</v>
+      <c r="B20" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="8" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1116,16 +1116,16 @@
       <c r="A21" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>10</v>
+      <c r="B21" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="8" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1133,16 +1133,16 @@
       <c r="A22" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>10</v>
+      <c r="B22" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="8" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1150,16 +1150,16 @@
       <c r="A23" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>10</v>
+      <c r="B23" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="8" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1167,16 +1167,16 @@
       <c r="A24" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>10</v>
+      <c r="B24" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="8" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1184,46 +1184,46 @@
       <c r="A25" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>10</v>
+      <c r="B25" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D25" s="14" t="str">
         <f>HYPERLINK("http://hl7.org/fhir/stu3/references.html","Reference")</f>
         <v>Reference</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="12"/>
-      <c r="B26" s="5"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D26" s="15" t="str">
         <f>HYPERLINK("https://fhir.hl7.org.uk/STU3/StructureDefinition/CareConnect-Organization-1","CareConnect-Organization-1")</f>
         <v>CareConnect-Organization-1</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="8"/>
     </row>
     <row r="27">
       <c r="A27" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>10</v>
+      <c r="B27" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="8" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1231,16 +1231,16 @@
       <c r="A28" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>10</v>
+      <c r="B28" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="8" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1248,857 +1248,857 @@
       <c r="A29" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>10</v>
+      <c r="B29" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>10</v>
+      <c r="B30" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="6" t="s">
         <v>84</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D31" s="14" t="str">
         <f>HYPERLINK("http://hl7.org/fhir/stu3/references.html","Reference")</f>
         <v>Reference</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="8" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="6"/>
       <c r="C32" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D32" s="15" t="str">
         <f>HYPERLINK("https://fhir.hl7.org.uk/STU3/StructureDefinition/CareConnect-Patient-1","CareConnect-Patient-1")</f>
         <v>CareConnect-Patient-1</v>
       </c>
-      <c r="E32" s="7"/>
+      <c r="E32" s="8"/>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>10</v>
+      <c r="B33" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>10</v>
+      <c r="B34" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>10</v>
+      <c r="B35" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>10</v>
+      <c r="B36" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="8" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>10</v>
+      <c r="B38" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>10</v>
+      <c r="B39" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E39" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>10</v>
+      <c r="B40" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E40" s="7" t="s">
+      <c r="E40" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>10</v>
+      <c r="B41" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E41" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>10</v>
+      <c r="B42" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>10</v>
+      <c r="B43" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D43" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="E43" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E44" s="8" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>10</v>
+      <c r="B45" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D45" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="E45" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>10</v>
+      <c r="B46" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E46" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>10</v>
+      <c r="B47" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D47" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="E47" s="8" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D48" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E48" s="8" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D49" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="8" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="E50" s="8" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>10</v>
+      <c r="B51" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D51" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="E51" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>10</v>
+      <c r="B52" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D52" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E52" s="7" t="s">
+      <c r="E52" s="8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>10</v>
+      <c r="B53" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D53" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="E53" s="8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D54" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="E54" s="8" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>10</v>
+      <c r="B55" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D55" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="E55" s="8" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>10</v>
+      <c r="B56" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D56" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="E56" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>10</v>
+      <c r="B57" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D57" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="E57" s="8" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>10</v>
+      <c r="B58" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D58" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="E58" s="7" t="s">
+      <c r="E58" s="8" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>10</v>
+      <c r="B59" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D59" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E59" s="7" t="s">
+      <c r="E59" s="8" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>10</v>
+      <c r="B60" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D60" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E60" s="7" t="s">
+      <c r="E60" s="8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>10</v>
+      <c r="B61" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D61" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E61" s="7" t="s">
+      <c r="E61" s="8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>10</v>
+      <c r="B62" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D62" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E62" s="7" t="s">
+      <c r="E62" s="8" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>10</v>
+      <c r="B63" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D63" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="E63" s="8" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D64" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="E64" s="7" t="s">
+      <c r="E64" s="8" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B65" s="5" t="s">
-        <v>10</v>
+      <c r="B65" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D65" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E65" s="7" t="s">
+      <c r="E65" s="8" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>10</v>
+      <c r="B66" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D66" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E66" s="7" t="s">
+      <c r="E66" s="8" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="4" t="s">
+      <c r="A67" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B67" s="5" t="s">
-        <v>10</v>
+      <c r="B67" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D67" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E67" s="7" t="s">
+      <c r="E67" s="8" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D68" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E68" s="7" t="s">
+      <c r="E68" s="8" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="4" t="s">
+      <c r="A69" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>10</v>
+      <c r="B69" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D69" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E69" s="7" t="s">
+      <c r="E69" s="8" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="4" t="s">
+      <c r="A70" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B70" s="5" t="s">
-        <v>10</v>
+      <c r="B70" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D70" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E70" s="7" t="s">
+      <c r="E70" s="8" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>10</v>
+      <c r="B71" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D71" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E71" s="7" t="s">
+      <c r="E71" s="8" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="4" t="s">
+      <c r="A72" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>10</v>
+      <c r="B72" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D72" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E72" s="7" t="s">
+      <c r="E72" s="8" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>10</v>
+      <c r="B73" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D73" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E73" s="7" t="s">
+      <c r="E73" s="8" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="4" t="s">
+      <c r="A74" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>10</v>
+      <c r="B74" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D74" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E74" s="7" t="s">
+      <c r="E74" s="8" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="4" t="s">
+      <c r="A75" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B75" s="5" t="s">
-        <v>10</v>
+      <c r="B75" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D75" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E75" s="7" t="s">
+      <c r="E75" s="8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="4" t="s">
+      <c r="A76" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B76" s="5" t="s">
-        <v>10</v>
+      <c r="B76" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D76" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E76" s="7" t="s">
+      <c r="E76" s="8" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="4" t="s">
+      <c r="A77" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D77" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="E77" s="7" t="s">
+      <c r="E77" s="8" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B78" s="5" t="s">
-        <v>10</v>
+      <c r="B78" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D78" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E78" s="7" t="s">
+      <c r="E78" s="8" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B79" s="5" t="s">
-        <v>10</v>
+      <c r="B79" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D79" s="10" t="s">
         <v>24</v>
@@ -2108,155 +2108,155 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="4" t="s">
+      <c r="A80" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="B80" s="5" t="s">
-        <v>10</v>
+      <c r="B80" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D80" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="E80" s="7" t="s">
+      <c r="E80" s="8" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B81" s="5" t="s">
-        <v>10</v>
+      <c r="B81" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D81" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E81" s="7" t="s">
+      <c r="E81" s="8" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="4" t="s">
+      <c r="A82" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B82" s="5" t="s">
-        <v>10</v>
+      <c r="B82" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D82" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="E82" s="7" t="s">
+      <c r="E82" s="8" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="4" t="s">
+      <c r="A83" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="B83" s="5" t="s">
-        <v>10</v>
+      <c r="B83" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D83" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="E83" s="7" t="s">
+      <c r="E83" s="8" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="4" t="s">
+      <c r="A84" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B84" s="5" t="s">
-        <v>10</v>
+      <c r="B84" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D84" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E84" s="7" t="s">
+      <c r="E84" s="8" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="4" t="s">
+      <c r="A85" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B85" s="5" t="s">
-        <v>10</v>
+      <c r="B85" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D85" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E85" s="7" t="s">
+      <c r="E85" s="8" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="4" t="s">
+      <c r="A86" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B86" s="5" t="s">
-        <v>10</v>
+      <c r="B86" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D86" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E86" s="7" t="s">
+      <c r="E86" s="8" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="4" t="s">
+      <c r="A87" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B87" s="5" t="s">
-        <v>10</v>
+      <c r="B87" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D87" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E87" s="7" t="s">
+      <c r="E87" s="8" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="4" t="s">
+      <c r="A88" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B88" s="5" t="s">
-        <v>10</v>
+      <c r="B88" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D88" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E88" s="7" t="s">
+      <c r="E88" s="8" t="s">
         <v>72</v>
       </c>
     </row>
@@ -8770,28 +8770,28 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
     <row r="4">
-      <c r="A4" s="8" t="s">
-        <v>13</v>
+      <c r="A4" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="s">
-        <v>14</v>
+      <c r="A5" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>